<commit_message>
add marking PNI data to enhancement folder
</commit_message>
<xml_diff>
--- a/data/enhancement-PNI/4Mile_mark_history.xlsx
+++ b/data/enhancement-PNI/4Mile_mark_history.xlsx
@@ -5,15 +5,16 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\DAVIDSONKA\Documents\ANALYSIS\San_Juan\data\enhancement-PNI\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\DAVIDSONKA\Documents\ANALYSIS\Area20\A20\data\enhancement-PNI\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E76D636E-2E69-4EBF-8CEF-84BFC5C76DC4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8035239A-C39F-415B-A971-663849105C36}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15990" xr2:uid="{DE54C1EF-7111-4456-8943-11E07DF116B0}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15525" activeTab="1" xr2:uid="{DE54C1EF-7111-4456-8943-11E07DF116B0}"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="old" sheetId="1" r:id="rId1"/>
+    <sheet name="PBT" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -36,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="44" uniqueCount="20">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="54" uniqueCount="21">
   <si>
     <t>% CWT</t>
   </si>
@@ -96,6 +97,9 @@
   </si>
   <si>
     <t>Marked – good</t>
+  </si>
+  <si>
+    <t>*Should be full soon</t>
   </si>
 </sst>
 </file>
@@ -471,8 +475,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B05E17FB-454E-45DC-8A73-09FA1DC08FD6}">
   <dimension ref="A1:G44"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
-      <selection activeCell="J41" sqref="J41"/>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:G1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1001,4 +1005,85 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{15F978E0-D613-4281-9D82-2D2CD6482AB5}">
+  <dimension ref="A1:C7"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="I11" sqref="I11"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="12.85546875" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>15</v>
+      </c>
+      <c r="B1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A2">
+        <v>2017</v>
+      </c>
+      <c r="B2" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A3">
+        <v>2018</v>
+      </c>
+      <c r="B3" t="s">
+        <v>8</v>
+      </c>
+      <c r="C3" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A4">
+        <v>2019</v>
+      </c>
+      <c r="B4" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A5">
+        <v>2020</v>
+      </c>
+      <c r="B5" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A6">
+        <v>2021</v>
+      </c>
+      <c r="B6" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A7">
+        <v>2022</v>
+      </c>
+      <c r="B7" t="s">
+        <v>10</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+</worksheet>
 </file>
</xml_diff>